<commit_message>
further developed the user interface
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/Orders.xlsx
+++ b/Project0/TempMohit/Data/Orders.xlsx
@@ -516,6 +516,17 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="2" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="n">
+        <x:v>126</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1089,6 +1100,35 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
+    <x:row r="20" spans="1:9">
+      <x:c r="A20" s="2" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B20" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D20" s="2" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E20" s="2" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="F20" s="2" t="n">
+        <x:v>0.4</x:v>
+      </x:c>
+      <x:c r="G20" s="2" t="n">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H20" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I20" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>